<commit_message>
Ajuste de esqueleto y de nombres cruzados de archivos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion13/EsqueletoGuion_CN_07_13_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion13/EsqueletoGuion_CN_07_13_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado07\guion13\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="12240" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="3408" yWindow="1395" windowWidth="19444" windowHeight="12244" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -19,18 +24,18 @@
   </definedNames>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="77">
   <si>
     <t>FICHA</t>
   </si>
@@ -257,17 +262,17 @@
     <t>Competencias</t>
   </si>
   <si>
-    <t>Fin de unidad</t>
-  </si>
-  <si>
     <t>Evaluación</t>
+  </si>
+  <si>
+    <t>Más información</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,7 +353,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,8 +384,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -401,6 +412,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="401">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -805,7 +831,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -872,13 +898,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1551,27 +1582,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +1610,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
@@ -1595,7 +1626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
@@ -1603,7 +1634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
@@ -1611,7 +1642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1631,26 +1662,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -1670,7 +1701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>6</v>
       </c>
@@ -1696,16 +1727,16 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G12" s="10"/>
     </row>
   </sheetData>
@@ -1720,20 +1751,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1744,7 +1775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1755,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1766,7 +1797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1777,7 +1808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1788,7 +1819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1799,7 +1830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1810,7 +1841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1821,7 +1852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1832,7 +1863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1843,7 +1874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1854,7 +1885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1865,7 +1896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1876,7 +1907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1887,7 +1918,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1898,7 +1929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1909,7 +1940,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1920,7 +1951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1931,7 +1962,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1942,7 +1973,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1953,7 +1984,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1964,9 +1995,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -1991,24 +2022,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -2019,7 +2050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2030,29 +2061,29 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2063,7 +2094,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2074,7 +2105,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2085,7 +2116,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2096,7 +2127,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2107,7 +2138,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2118,7 +2149,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2129,7 +2160,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2140,7 +2171,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2151,7 +2182,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2162,7 +2193,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2173,7 +2204,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2184,7 +2215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2195,7 +2226,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2206,7 +2237,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2217,7 +2248,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2228,7 +2259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2239,7 +2270,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2250,18 +2281,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C28" s="6"/>
     </row>
   </sheetData>
@@ -2280,28 +2311,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B86" sqref="B86:B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="43.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.59765625" style="2" customWidth="1"/>
     <col min="3" max="3" width="21" style="2" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="52.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.19921875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.1328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="52.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75">
+    <row r="1" spans="1:11" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -2330,7 +2361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2346,7 +2377,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2362,7 +2393,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2378,7 +2409,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2401,7 +2432,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="23" t="s">
         <v>19</v>
       </c>
@@ -2420,7 +2451,7 @@
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="23" t="s">
         <v>19</v>
       </c>
@@ -2443,7 +2474,7 @@
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="23" t="s">
         <v>19</v>
       </c>
@@ -2464,7 +2495,7 @@
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="23" t="s">
         <v>19</v>
       </c>
@@ -2485,7 +2516,7 @@
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="23" t="s">
         <v>19</v>
       </c>
@@ -2504,7 +2535,7 @@
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="23" t="s">
         <v>19</v>
       </c>
@@ -2516,7 +2547,7 @@
         <v>57</v>
       </c>
       <c r="E11" s="29"/>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="33" t="s">
         <v>58</v>
       </c>
       <c r="G11" s="29" t="s">
@@ -2525,7 +2556,7 @@
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
@@ -2537,7 +2568,7 @@
         <v>57</v>
       </c>
       <c r="E12" s="29"/>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="33" t="s">
         <v>58</v>
       </c>
       <c r="G12" s="29" t="s">
@@ -2546,7 +2577,7 @@
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="23" t="s">
         <v>19</v>
       </c>
@@ -2558,7 +2589,7 @@
         <v>57</v>
       </c>
       <c r="E13" s="29"/>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="33" t="s">
         <v>58</v>
       </c>
       <c r="G13" s="29" t="s">
@@ -2567,7 +2598,7 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="23" t="s">
         <v>19</v>
       </c>
@@ -2579,7 +2610,7 @@
         <v>57</v>
       </c>
       <c r="E14" s="29"/>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="33" t="s">
         <v>58</v>
       </c>
       <c r="G14" s="29" t="s">
@@ -2588,7 +2619,7 @@
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="23" t="s">
         <v>19</v>
       </c>
@@ -2600,7 +2631,7 @@
         <v>57</v>
       </c>
       <c r="E15" s="29"/>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="33" t="s">
         <v>58</v>
       </c>
       <c r="G15" s="29" t="s">
@@ -2609,7 +2640,7 @@
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="23" t="s">
         <v>19</v>
       </c>
@@ -2621,7 +2652,7 @@
         <v>57</v>
       </c>
       <c r="E16" s="29"/>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="33" t="s">
         <v>58</v>
       </c>
       <c r="G16" s="29" t="s">
@@ -2630,7 +2661,7 @@
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
     </row>
-    <row r="17" spans="1:24" ht="15" customHeight="1">
+    <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="23" t="s">
         <v>19</v>
       </c>
@@ -2642,7 +2673,7 @@
         <v>57</v>
       </c>
       <c r="E17" s="29"/>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="33" t="s">
         <v>58</v>
       </c>
       <c r="G17" s="29" t="s">
@@ -2651,7 +2682,7 @@
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" spans="1:24" ht="15" customHeight="1">
+    <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="23" t="s">
         <v>19</v>
       </c>
@@ -2663,7 +2694,7 @@
         <v>57</v>
       </c>
       <c r="E18" s="29"/>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="33" t="s">
         <v>58</v>
       </c>
       <c r="G18" s="29" t="s">
@@ -2676,7 +2707,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15" customHeight="1">
+    <row r="19" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="23" t="s">
         <v>19</v>
       </c>
@@ -2688,7 +2719,7 @@
         <v>57</v>
       </c>
       <c r="E19" s="29"/>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="33" t="s">
         <v>58</v>
       </c>
       <c r="G19" s="29" t="s">
@@ -2701,7 +2732,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="12.75" customHeight="1">
+    <row r="20" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="23" t="s">
         <v>19</v>
       </c>
@@ -2722,7 +2753,7 @@
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
     </row>
-    <row r="21" spans="1:24" ht="18" customHeight="1">
+    <row r="21" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="23" t="s">
         <v>19</v>
       </c>
@@ -2743,7 +2774,7 @@
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
     </row>
-    <row r="22" spans="1:24" ht="18" customHeight="1">
+    <row r="22" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="23" t="s">
         <v>19</v>
       </c>
@@ -2764,7 +2795,7 @@
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
     </row>
-    <row r="23" spans="1:24" ht="18" customHeight="1">
+    <row r="23" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="23" t="s">
         <v>19</v>
       </c>
@@ -2785,7 +2816,7 @@
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
     </row>
-    <row r="24" spans="1:24" ht="18" customHeight="1">
+    <row r="24" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="23" t="s">
         <v>19</v>
       </c>
@@ -2806,7 +2837,7 @@
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
     </row>
-    <row r="25" spans="1:24" ht="18" customHeight="1">
+    <row r="25" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="23" t="s">
         <v>19</v>
       </c>
@@ -2827,7 +2858,7 @@
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
     </row>
-    <row r="26" spans="1:24" ht="18" customHeight="1">
+    <row r="26" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="23" t="s">
         <v>19</v>
       </c>
@@ -2848,7 +2879,7 @@
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
     </row>
-    <row r="27" spans="1:24" ht="18" customHeight="1">
+    <row r="27" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="23" t="s">
         <v>19</v>
       </c>
@@ -2873,7 +2904,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A28" s="23" t="s">
         <v>19</v>
       </c>
@@ -2896,7 +2927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A29" s="24" t="s">
         <v>19</v>
       </c>
@@ -2928,7 +2959,7 @@
       <c r="W29" s="24"/>
       <c r="X29" s="24"/>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A30" s="24" t="s">
         <v>19</v>
       </c>
@@ -2960,7 +2991,7 @@
       <c r="W30" s="24"/>
       <c r="X30" s="24"/>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
@@ -2994,7 +3025,7 @@
       <c r="W31" s="24"/>
       <c r="X31" s="24"/>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A32" s="24" t="s">
         <v>19</v>
       </c>
@@ -3028,7 +3059,7 @@
       <c r="W32" s="24"/>
       <c r="X32" s="24"/>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A33" s="24" t="s">
         <v>19</v>
       </c>
@@ -3062,7 +3093,7 @@
       <c r="W33" s="24"/>
       <c r="X33" s="24"/>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A34" s="24" t="s">
         <v>19</v>
       </c>
@@ -3096,7 +3127,7 @@
       <c r="W34" s="24"/>
       <c r="X34" s="24"/>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A35" s="24" t="s">
         <v>19</v>
       </c>
@@ -3130,7 +3161,7 @@
       <c r="W35" s="24"/>
       <c r="X35" s="24"/>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A36" s="24" t="s">
         <v>19</v>
       </c>
@@ -3164,7 +3195,7 @@
       <c r="W36" s="24"/>
       <c r="X36" s="24"/>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A37" s="24" t="s">
         <v>19</v>
       </c>
@@ -3198,7 +3229,7 @@
       <c r="W37" s="24"/>
       <c r="X37" s="24"/>
     </row>
-    <row r="38" spans="1:24">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A38" s="24" t="s">
         <v>19</v>
       </c>
@@ -3232,7 +3263,7 @@
       <c r="W38" s="24"/>
       <c r="X38" s="24"/>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A39" s="24" t="s">
         <v>19</v>
       </c>
@@ -3270,7 +3301,7 @@
       <c r="W39" s="24"/>
       <c r="X39" s="24"/>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A40" s="24" t="s">
         <v>19</v>
       </c>
@@ -3304,7 +3335,7 @@
       <c r="W40" s="24"/>
       <c r="X40" s="24"/>
     </row>
-    <row r="41" spans="1:24">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A41" s="24" t="s">
         <v>19</v>
       </c>
@@ -3342,7 +3373,7 @@
       <c r="W41" s="24"/>
       <c r="X41" s="24"/>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A42" s="24" t="s">
         <v>19</v>
       </c>
@@ -3376,7 +3407,7 @@
       <c r="W42" s="24"/>
       <c r="X42" s="24"/>
     </row>
-    <row r="43" spans="1:24">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A43" s="24" t="s">
         <v>19</v>
       </c>
@@ -3387,7 +3418,7 @@
       <c r="D43" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="34" t="s">
+      <c r="E43" s="32" t="s">
         <v>54</v>
       </c>
       <c r="F43" s="25"/>
@@ -3414,7 +3445,7 @@
       <c r="W43" s="24"/>
       <c r="X43" s="24"/>
     </row>
-    <row r="44" spans="1:24">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A44" s="21" t="s">
         <v>19</v>
       </c>
@@ -3434,7 +3465,7 @@
       <c r="K44" s="18"/>
       <c r="L44" s="18"/>
     </row>
-    <row r="45" spans="1:24">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A45" s="21" t="s">
         <v>19</v>
       </c>
@@ -3456,7 +3487,7 @@
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
     </row>
-    <row r="46" spans="1:24">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A46" s="21" t="s">
         <v>19</v>
       </c>
@@ -3478,7 +3509,7 @@
       <c r="K46" s="18"/>
       <c r="L46" s="18"/>
     </row>
-    <row r="47" spans="1:24">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A47" s="21" t="s">
         <v>19</v>
       </c>
@@ -3500,7 +3531,7 @@
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A48" s="21" t="s">
         <v>19</v>
       </c>
@@ -3522,7 +3553,7 @@
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="21" t="s">
         <v>19</v>
       </c>
@@ -3544,7 +3575,7 @@
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="21" t="s">
         <v>19</v>
       </c>
@@ -3566,7 +3597,7 @@
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
@@ -3588,7 +3619,7 @@
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" s="21" t="s">
         <v>19</v>
       </c>
@@ -3610,7 +3641,7 @@
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" s="21" t="s">
         <v>19</v>
       </c>
@@ -3632,7 +3663,7 @@
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="21" t="s">
         <v>19</v>
       </c>
@@ -3654,7 +3685,7 @@
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="21" t="s">
         <v>19</v>
       </c>
@@ -3676,7 +3707,7 @@
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="21" t="s">
         <v>19</v>
       </c>
@@ -3698,7 +3729,7 @@
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" s="21" t="s">
         <v>19</v>
       </c>
@@ -3720,7 +3751,7 @@
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" s="21" t="s">
         <v>19</v>
       </c>
@@ -3746,7 +3777,7 @@
       <c r="K58" s="18"/>
       <c r="L58" s="18"/>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A59" s="21" t="s">
         <v>19</v>
       </c>
@@ -3768,7 +3799,7 @@
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60" s="21" t="s">
         <v>19</v>
       </c>
@@ -3790,7 +3821,7 @@
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A61" s="21" t="s">
         <v>19</v>
       </c>
@@ -3812,7 +3843,7 @@
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62" s="21" t="s">
         <v>19</v>
       </c>
@@ -3834,7 +3865,7 @@
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" s="21" t="s">
         <v>19</v>
       </c>
@@ -3860,7 +3891,7 @@
       <c r="K63" s="18"/>
       <c r="L63" s="18"/>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" s="21" t="s">
         <v>19</v>
       </c>
@@ -3886,7 +3917,7 @@
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A65" s="18" t="s">
         <v>19</v>
       </c>
@@ -3898,7 +3929,7 @@
       </c>
       <c r="D65" s="19"/>
       <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
+      <c r="F65" s="34"/>
       <c r="G65" s="19"/>
       <c r="H65" s="18"/>
       <c r="I65" s="17"/>
@@ -3910,7 +3941,7 @@
       <c r="O65" s="18"/>
       <c r="P65" s="18"/>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A66" s="18" t="s">
         <v>19</v>
       </c>
@@ -3924,7 +3955,7 @@
       <c r="E66" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F66" s="32"/>
+      <c r="F66" s="35"/>
       <c r="G66" s="19"/>
       <c r="H66" s="18"/>
       <c r="I66" s="17"/>
@@ -3936,7 +3967,7 @@
       <c r="O66" s="18"/>
       <c r="P66" s="18"/>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A67" s="18" t="s">
         <v>19</v>
       </c>
@@ -3948,7 +3979,7 @@
         <v>41</v>
       </c>
       <c r="E67" s="19"/>
-      <c r="F67" s="32" t="s">
+      <c r="F67" s="35" t="s">
         <v>71</v>
       </c>
       <c r="G67" s="19" t="s">
@@ -3964,7 +3995,7 @@
       <c r="O67" s="18"/>
       <c r="P67" s="18"/>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A68" s="18" t="s">
         <v>19</v>
       </c>
@@ -3976,7 +4007,7 @@
         <v>41</v>
       </c>
       <c r="E68" s="19"/>
-      <c r="F68" s="32" t="s">
+      <c r="F68" s="35" t="s">
         <v>71</v>
       </c>
       <c r="G68" s="19" t="s">
@@ -3992,7 +4023,7 @@
       <c r="O68" s="18"/>
       <c r="P68" s="18"/>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A69" s="18" t="s">
         <v>19</v>
       </c>
@@ -4004,7 +4035,7 @@
         <v>41</v>
       </c>
       <c r="E69" s="19"/>
-      <c r="F69" s="33" t="s">
+      <c r="F69" s="36" t="s">
         <v>72</v>
       </c>
       <c r="G69" s="17" t="s">
@@ -4020,7 +4051,7 @@
       <c r="O69" s="18"/>
       <c r="P69" s="18"/>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A70" s="18" t="s">
         <v>19</v>
       </c>
@@ -4032,7 +4063,7 @@
         <v>41</v>
       </c>
       <c r="E70" s="19"/>
-      <c r="F70" s="33" t="s">
+      <c r="F70" s="36" t="s">
         <v>72</v>
       </c>
       <c r="G70" s="17" t="s">
@@ -4052,7 +4083,7 @@
       <c r="O70" s="18"/>
       <c r="P70" s="18"/>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A71" s="18" t="s">
         <v>19</v>
       </c>
@@ -4066,7 +4097,7 @@
       <c r="E71" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F71" s="19"/>
+      <c r="F71" s="34"/>
       <c r="G71" s="19"/>
       <c r="H71" s="18"/>
       <c r="I71" s="17"/>
@@ -4078,7 +4109,7 @@
       <c r="O71" s="18"/>
       <c r="P71" s="18"/>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A72" s="18" t="s">
         <v>19</v>
       </c>
@@ -4092,7 +4123,7 @@
       <c r="E72" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F72" s="19"/>
+      <c r="F72" s="34"/>
       <c r="G72" s="19"/>
       <c r="H72" s="18"/>
       <c r="I72" s="17"/>
@@ -4104,7 +4135,7 @@
       <c r="O72" s="18"/>
       <c r="P72" s="18"/>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A73" s="18" t="s">
         <v>19</v>
       </c>
@@ -4130,7 +4161,7 @@
       <c r="O73" s="18"/>
       <c r="P73" s="18"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A74" s="18" t="s">
         <v>19</v>
       </c>
@@ -4156,7 +4187,7 @@
       <c r="O74" s="18"/>
       <c r="P74" s="18"/>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A75" s="18" t="s">
         <v>19</v>
       </c>
@@ -4182,7 +4213,7 @@
       <c r="O75" s="18"/>
       <c r="P75" s="18"/>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A76" s="18" t="s">
         <v>19</v>
       </c>
@@ -4208,7 +4239,7 @@
       <c r="O76" s="18"/>
       <c r="P76" s="18"/>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A77" s="18" t="s">
         <v>19</v>
       </c>
@@ -4234,7 +4265,7 @@
       <c r="O77" s="18"/>
       <c r="P77" s="18"/>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A78" s="18" t="s">
         <v>19</v>
       </c>
@@ -4264,7 +4295,7 @@
       <c r="O78" s="18"/>
       <c r="P78" s="18"/>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A79" s="18" t="s">
         <v>19</v>
       </c>
@@ -4290,7 +4321,7 @@
       <c r="O79" s="18"/>
       <c r="P79" s="18"/>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A80" s="18" t="s">
         <v>19</v>
       </c>
@@ -4320,7 +4351,7 @@
       <c r="O80" s="18"/>
       <c r="P80" s="18"/>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>19</v>
       </c>
@@ -4337,7 +4368,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>19</v>
       </c>
@@ -4354,7 +4385,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
         <v>19</v>
       </c>
@@ -4371,7 +4402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
         <v>19</v>
       </c>
@@ -4388,7 +4419,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
         <v>19</v>
       </c>
@@ -4405,48 +4436,48 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C86" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="37"/>
+      <c r="G86" s="37"/>
+      <c r="H86" s="37"/>
+      <c r="I86" s="37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A87" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C87" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C86" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D86" s="19"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="19"/>
-      <c r="G86" s="19"/>
-      <c r="H86" s="18"/>
-      <c r="I86" s="17"/>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B87" s="18" t="s">
+      <c r="D87" s="37"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="37"/>
+      <c r="H87" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C87" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D87" s="19"/>
-      <c r="E87" s="19"/>
-      <c r="F87" s="19"/>
-      <c r="G87" s="19"/>
-      <c r="H87" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="I87" s="17" t="s">
+      <c r="I87" s="37" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I87">
-    <filterColumn colId="8"/>
-  </autoFilter>
+  <autoFilter ref="A1:I87"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>

</xml_diff>

<commit_message>
Versión original después de corrección de estilo.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion13/EsqueletoGuion_CN_07_13_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion13/EsqueletoGuion_CN_07_13_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado07\guion13\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3408" yWindow="1395" windowWidth="19444" windowHeight="12244" tabRatio="729"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -23,8 +18,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'RECURSOS NUEVOS'!$A$1:$C$22</definedName>
   </definedNames>
   <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -271,8 +266,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1582,27 +1577,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
@@ -1610,7 +1605,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2">
       <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
@@ -1618,7 +1613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2">
       <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
@@ -1626,7 +1621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2">
       <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
@@ -1634,7 +1629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2">
       <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
@@ -1642,7 +1637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1662,26 +1657,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.73046875" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -1701,7 +1696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="4" customFormat="1">
       <c r="A2">
         <v>6</v>
       </c>
@@ -1727,16 +1722,16 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12">
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12">
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12">
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12">
       <c r="G12" s="10"/>
     </row>
   </sheetData>
@@ -1751,20 +1746,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="66.1328125" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" customWidth="1"/>
+    <col min="1" max="1" width="66.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" s="4" customFormat="1">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1786,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" s="4" customFormat="1">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1797,7 +1792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" s="4" customFormat="1">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1808,7 +1803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" s="4" customFormat="1">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1819,7 +1814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1830,7 +1825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1841,7 +1836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1852,7 +1847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1863,7 +1858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1874,7 +1869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1885,7 +1880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1896,7 +1891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1907,7 +1902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1918,7 +1913,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1929,7 +1924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1940,7 +1935,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1951,7 +1946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1962,7 +1957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1973,7 +1968,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1984,7 +1979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1995,7 +1990,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -2022,7 +2017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2032,14 +2027,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="92.265625" customWidth="1"/>
-    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -2050,7 +2045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2061,7 +2056,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2072,7 +2067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2083,7 +2078,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2094,7 +2089,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2105,7 +2100,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2116,7 +2111,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2127,7 +2122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2138,7 +2133,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2149,7 +2144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2160,7 +2155,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2171,7 +2166,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2182,7 +2177,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2193,7 +2188,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2204,7 +2199,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2215,7 +2210,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2226,7 +2221,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2237,7 +2232,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2248,7 +2243,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2259,7 +2254,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2270,7 +2265,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2281,7 +2276,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2292,7 +2287,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3">
       <c r="C28" s="6"/>
     </row>
   </sheetData>
@@ -2311,28 +2306,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X87"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B86" sqref="B86:B87"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.59765625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="21" style="2" customWidth="1"/>
-    <col min="4" max="4" width="59.19921875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.86328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.1328125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.86328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="52.1328125" customWidth="1"/>
-    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="52.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -2361,7 +2356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2377,7 +2372,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2393,7 +2388,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2409,7 +2404,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2432,7 +2427,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11">
       <c r="A6" s="23" t="s">
         <v>19</v>
       </c>
@@ -2451,7 +2446,7 @@
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11">
       <c r="A7" s="23" t="s">
         <v>19</v>
       </c>
@@ -2474,7 +2469,7 @@
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="15" customHeight="1">
       <c r="A8" s="23" t="s">
         <v>19</v>
       </c>
@@ -2495,7 +2490,7 @@
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="15" customHeight="1">
       <c r="A9" s="23" t="s">
         <v>19</v>
       </c>
@@ -2516,7 +2511,7 @@
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="23" t="s">
         <v>19</v>
       </c>
@@ -2535,7 +2530,7 @@
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="A11" s="23" t="s">
         <v>19</v>
       </c>
@@ -2556,7 +2551,7 @@
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" ht="15" customHeight="1">
       <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
@@ -2577,7 +2572,7 @@
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" ht="15" customHeight="1">
       <c r="A13" s="23" t="s">
         <v>19</v>
       </c>
@@ -2598,7 +2593,7 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" ht="15" customHeight="1">
       <c r="A14" s="23" t="s">
         <v>19</v>
       </c>
@@ -2619,7 +2614,7 @@
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" ht="15" customHeight="1">
       <c r="A15" s="23" t="s">
         <v>19</v>
       </c>
@@ -2640,7 +2635,7 @@
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" ht="15" customHeight="1">
       <c r="A16" s="23" t="s">
         <v>19</v>
       </c>
@@ -2661,7 +2656,7 @@
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
     </row>
-    <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:24" ht="15" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>19</v>
       </c>
@@ -2682,7 +2677,7 @@
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:24" ht="15" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>19</v>
       </c>
@@ -2707,7 +2702,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:24" ht="15" customHeight="1">
       <c r="A19" s="23" t="s">
         <v>19</v>
       </c>
@@ -2732,7 +2727,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:24" ht="12.75" customHeight="1">
       <c r="A20" s="23" t="s">
         <v>19</v>
       </c>
@@ -2753,7 +2748,7 @@
       <c r="H20" s="28"/>
       <c r="I20" s="28"/>
     </row>
-    <row r="21" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:24" ht="18" customHeight="1">
       <c r="A21" s="23" t="s">
         <v>19</v>
       </c>
@@ -2774,7 +2769,7 @@
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
     </row>
-    <row r="22" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:24" ht="18" customHeight="1">
       <c r="A22" s="23" t="s">
         <v>19</v>
       </c>
@@ -2795,7 +2790,7 @@
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
     </row>
-    <row r="23" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:24" ht="18" customHeight="1">
       <c r="A23" s="23" t="s">
         <v>19</v>
       </c>
@@ -2816,7 +2811,7 @@
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
     </row>
-    <row r="24" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:24" ht="18" customHeight="1">
       <c r="A24" s="23" t="s">
         <v>19</v>
       </c>
@@ -2837,7 +2832,7 @@
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
     </row>
-    <row r="25" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:24" ht="18" customHeight="1">
       <c r="A25" s="23" t="s">
         <v>19</v>
       </c>
@@ -2858,7 +2853,7 @@
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
     </row>
-    <row r="26" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:24" ht="18" customHeight="1">
       <c r="A26" s="23" t="s">
         <v>19</v>
       </c>
@@ -2879,7 +2874,7 @@
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
     </row>
-    <row r="27" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:24" ht="18" customHeight="1">
       <c r="A27" s="23" t="s">
         <v>19</v>
       </c>
@@ -2904,7 +2899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:24">
       <c r="A28" s="23" t="s">
         <v>19</v>
       </c>
@@ -2927,7 +2922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:24">
       <c r="A29" s="24" t="s">
         <v>19</v>
       </c>
@@ -2959,7 +2954,7 @@
       <c r="W29" s="24"/>
       <c r="X29" s="24"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:24">
       <c r="A30" s="24" t="s">
         <v>19</v>
       </c>
@@ -2991,7 +2986,7 @@
       <c r="W30" s="24"/>
       <c r="X30" s="24"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:24">
       <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
@@ -3025,7 +3020,7 @@
       <c r="W31" s="24"/>
       <c r="X31" s="24"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:24">
       <c r="A32" s="24" t="s">
         <v>19</v>
       </c>
@@ -3059,7 +3054,7 @@
       <c r="W32" s="24"/>
       <c r="X32" s="24"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:24">
       <c r="A33" s="24" t="s">
         <v>19</v>
       </c>
@@ -3093,7 +3088,7 @@
       <c r="W33" s="24"/>
       <c r="X33" s="24"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:24">
       <c r="A34" s="24" t="s">
         <v>19</v>
       </c>
@@ -3127,7 +3122,7 @@
       <c r="W34" s="24"/>
       <c r="X34" s="24"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:24">
       <c r="A35" s="24" t="s">
         <v>19</v>
       </c>
@@ -3161,7 +3156,7 @@
       <c r="W35" s="24"/>
       <c r="X35" s="24"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:24">
       <c r="A36" s="24" t="s">
         <v>19</v>
       </c>
@@ -3195,7 +3190,7 @@
       <c r="W36" s="24"/>
       <c r="X36" s="24"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:24">
       <c r="A37" s="24" t="s">
         <v>19</v>
       </c>
@@ -3229,7 +3224,7 @@
       <c r="W37" s="24"/>
       <c r="X37" s="24"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:24">
       <c r="A38" s="24" t="s">
         <v>19</v>
       </c>
@@ -3263,7 +3258,7 @@
       <c r="W38" s="24"/>
       <c r="X38" s="24"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:24">
       <c r="A39" s="24" t="s">
         <v>19</v>
       </c>
@@ -3301,7 +3296,7 @@
       <c r="W39" s="24"/>
       <c r="X39" s="24"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:24">
       <c r="A40" s="24" t="s">
         <v>19</v>
       </c>
@@ -3335,7 +3330,7 @@
       <c r="W40" s="24"/>
       <c r="X40" s="24"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:24">
       <c r="A41" s="24" t="s">
         <v>19</v>
       </c>
@@ -3373,7 +3368,7 @@
       <c r="W41" s="24"/>
       <c r="X41" s="24"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:24">
       <c r="A42" s="24" t="s">
         <v>19</v>
       </c>
@@ -3407,7 +3402,7 @@
       <c r="W42" s="24"/>
       <c r="X42" s="24"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:24">
       <c r="A43" s="24" t="s">
         <v>19</v>
       </c>
@@ -3445,7 +3440,7 @@
       <c r="W43" s="24"/>
       <c r="X43" s="24"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:24">
       <c r="A44" s="21" t="s">
         <v>19</v>
       </c>
@@ -3465,7 +3460,7 @@
       <c r="K44" s="18"/>
       <c r="L44" s="18"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:24">
       <c r="A45" s="21" t="s">
         <v>19</v>
       </c>
@@ -3487,7 +3482,7 @@
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:24">
       <c r="A46" s="21" t="s">
         <v>19</v>
       </c>
@@ -3509,7 +3504,7 @@
       <c r="K46" s="18"/>
       <c r="L46" s="18"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:24">
       <c r="A47" s="21" t="s">
         <v>19</v>
       </c>
@@ -3531,7 +3526,7 @@
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:24">
       <c r="A48" s="21" t="s">
         <v>19</v>
       </c>
@@ -3553,7 +3548,7 @@
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12">
       <c r="A49" s="21" t="s">
         <v>19</v>
       </c>
@@ -3575,7 +3570,7 @@
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12">
       <c r="A50" s="21" t="s">
         <v>19</v>
       </c>
@@ -3597,7 +3592,7 @@
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
@@ -3619,7 +3614,7 @@
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12">
       <c r="A52" s="21" t="s">
         <v>19</v>
       </c>
@@ -3641,7 +3636,7 @@
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12">
       <c r="A53" s="21" t="s">
         <v>19</v>
       </c>
@@ -3663,7 +3658,7 @@
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12">
       <c r="A54" s="21" t="s">
         <v>19</v>
       </c>
@@ -3685,7 +3680,7 @@
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12">
       <c r="A55" s="21" t="s">
         <v>19</v>
       </c>
@@ -3707,7 +3702,7 @@
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12">
       <c r="A56" s="21" t="s">
         <v>19</v>
       </c>
@@ -3729,7 +3724,7 @@
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:12">
       <c r="A57" s="21" t="s">
         <v>19</v>
       </c>
@@ -3751,7 +3746,7 @@
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:12">
       <c r="A58" s="21" t="s">
         <v>19</v>
       </c>
@@ -3777,7 +3772,7 @@
       <c r="K58" s="18"/>
       <c r="L58" s="18"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:12">
       <c r="A59" s="21" t="s">
         <v>19</v>
       </c>
@@ -3799,7 +3794,7 @@
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:12">
       <c r="A60" s="21" t="s">
         <v>19</v>
       </c>
@@ -3821,7 +3816,7 @@
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12">
       <c r="A61" s="21" t="s">
         <v>19</v>
       </c>
@@ -3843,7 +3838,7 @@
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12">
       <c r="A62" s="21" t="s">
         <v>19</v>
       </c>
@@ -3865,7 +3860,7 @@
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:12">
       <c r="A63" s="21" t="s">
         <v>19</v>
       </c>
@@ -3891,7 +3886,7 @@
       <c r="K63" s="18"/>
       <c r="L63" s="18"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:12">
       <c r="A64" s="21" t="s">
         <v>19</v>
       </c>
@@ -3917,7 +3912,7 @@
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:16">
       <c r="A65" s="18" t="s">
         <v>19</v>
       </c>
@@ -3941,7 +3936,7 @@
       <c r="O65" s="18"/>
       <c r="P65" s="18"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:16">
       <c r="A66" s="18" t="s">
         <v>19</v>
       </c>
@@ -3967,7 +3962,7 @@
       <c r="O66" s="18"/>
       <c r="P66" s="18"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:16">
       <c r="A67" s="18" t="s">
         <v>19</v>
       </c>
@@ -3995,7 +3990,7 @@
       <c r="O67" s="18"/>
       <c r="P67" s="18"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:16">
       <c r="A68" s="18" t="s">
         <v>19</v>
       </c>
@@ -4023,7 +4018,7 @@
       <c r="O68" s="18"/>
       <c r="P68" s="18"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:16">
       <c r="A69" s="18" t="s">
         <v>19</v>
       </c>
@@ -4051,7 +4046,7 @@
       <c r="O69" s="18"/>
       <c r="P69" s="18"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:16">
       <c r="A70" s="18" t="s">
         <v>19</v>
       </c>
@@ -4083,7 +4078,7 @@
       <c r="O70" s="18"/>
       <c r="P70" s="18"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:16">
       <c r="A71" s="18" t="s">
         <v>19</v>
       </c>
@@ -4109,7 +4104,7 @@
       <c r="O71" s="18"/>
       <c r="P71" s="18"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:16">
       <c r="A72" s="18" t="s">
         <v>19</v>
       </c>
@@ -4135,7 +4130,7 @@
       <c r="O72" s="18"/>
       <c r="P72" s="18"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:16">
       <c r="A73" s="18" t="s">
         <v>19</v>
       </c>
@@ -4161,7 +4156,7 @@
       <c r="O73" s="18"/>
       <c r="P73" s="18"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:16">
       <c r="A74" s="18" t="s">
         <v>19</v>
       </c>
@@ -4187,7 +4182,7 @@
       <c r="O74" s="18"/>
       <c r="P74" s="18"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:16">
       <c r="A75" s="18" t="s">
         <v>19</v>
       </c>
@@ -4213,7 +4208,7 @@
       <c r="O75" s="18"/>
       <c r="P75" s="18"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:16">
       <c r="A76" s="18" t="s">
         <v>19</v>
       </c>
@@ -4239,7 +4234,7 @@
       <c r="O76" s="18"/>
       <c r="P76" s="18"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:16">
       <c r="A77" s="18" t="s">
         <v>19</v>
       </c>
@@ -4265,7 +4260,7 @@
       <c r="O77" s="18"/>
       <c r="P77" s="18"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:16">
       <c r="A78" s="18" t="s">
         <v>19</v>
       </c>
@@ -4295,7 +4290,7 @@
       <c r="O78" s="18"/>
       <c r="P78" s="18"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:16">
       <c r="A79" s="18" t="s">
         <v>19</v>
       </c>
@@ -4321,7 +4316,7 @@
       <c r="O79" s="18"/>
       <c r="P79" s="18"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:16">
       <c r="A80" s="18" t="s">
         <v>19</v>
       </c>
@@ -4351,7 +4346,7 @@
       <c r="O80" s="18"/>
       <c r="P80" s="18"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9">
       <c r="A81" s="2" t="s">
         <v>19</v>
       </c>
@@ -4368,7 +4363,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9">
       <c r="A82" s="2" t="s">
         <v>19</v>
       </c>
@@ -4385,7 +4380,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9">
       <c r="A83" s="2" t="s">
         <v>19</v>
       </c>
@@ -4402,7 +4397,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9">
       <c r="A84" s="2" t="s">
         <v>19</v>
       </c>
@@ -4419,7 +4414,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9">
       <c r="A85" s="2" t="s">
         <v>19</v>
       </c>
@@ -4436,7 +4431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9">
       <c r="A86" s="18" t="s">
         <v>19</v>
       </c>
@@ -4455,7 +4450,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9">
       <c r="A87" s="18" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Adición nuevas filas (resaltadas en amarillo)
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion13/EsqueletoGuion_CN_07_13_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion13/EsqueletoGuion_CN_07_13_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado07\guion13\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" firstSheet="2" activeTab="4"/>
   </bookViews>
@@ -14,12 +19,12 @@
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CUADERNO DE ESTUDIO'!$A$1:$I$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CUADERNO DE ESTUDIO'!$A$1:$I$93</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'RECURSOS NUEVOS'!$A$1:$C$22</definedName>
   </definedNames>
   <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="77">
   <si>
     <t>FICHA</t>
   </si>
@@ -266,8 +271,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,7 +831,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -905,6 +910,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1577,27 +1594,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
@@ -1605,7 +1622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
@@ -1613,7 +1630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
@@ -1621,7 +1638,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
@@ -1629,7 +1646,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
@@ -1637,7 +1654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1657,14 +1674,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
@@ -1676,7 +1693,7 @@
     <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -1696,7 +1713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -1722,16 +1739,16 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G12" s="10"/>
     </row>
   </sheetData>
@@ -1746,20 +1763,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.140625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1770,7 +1787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1781,7 +1798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1792,7 +1809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1803,7 +1820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1814,7 +1831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1825,7 +1842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1836,7 +1853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1847,7 +1864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1858,7 +1875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1869,7 +1886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1880,7 +1897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1891,7 +1908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1902,7 +1919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1913,7 +1930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1924,7 +1941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1935,7 +1952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1946,7 +1963,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1957,7 +1974,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1968,7 +1985,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1979,7 +1996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1990,7 +2007,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -2017,7 +2034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2027,14 +2044,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="92.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -2045,7 +2062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2056,7 +2073,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2067,7 +2084,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2078,7 +2095,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2089,7 +2106,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2100,7 +2117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2111,7 +2128,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2122,7 +2139,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2133,7 +2150,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2144,7 +2161,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2155,7 +2172,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2166,7 +2183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2177,7 +2194,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2188,7 +2205,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2199,7 +2216,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2210,7 +2227,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2221,7 +2238,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2232,7 +2249,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2243,7 +2260,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2254,7 +2271,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2265,7 +2282,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2276,7 +2293,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2287,7 +2304,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" s="6"/>
     </row>
   </sheetData>
@@ -2306,15 +2323,15 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D88" sqref="A87:D88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.5703125" style="2" customWidth="1"/>
@@ -2327,7 +2344,7 @@
     <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -2356,7 +2373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2372,7 +2389,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2388,7 +2405,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2404,49 +2421,48 @@
       <c r="G4" s="9"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>54</v>
+      <c r="E5" s="42" t="s">
+        <v>51</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="I6" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>19</v>
       </c>
@@ -2454,43 +2470,41 @@
         <v>55</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
       <c r="G7" s="29"/>
-      <c r="H7" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="28" t="s">
-        <v>29</v>
-      </c>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>51</v>
-      </c>
+      <c r="C8" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
+      <c r="H8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>29</v>
+      </c>
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>19</v>
       </c>
@@ -2502,7 +2516,7 @@
         <v>57</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
@@ -2511,7 +2525,7 @@
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>19</v>
       </c>
@@ -2519,18 +2533,20 @@
         <v>55</v>
       </c>
       <c r="C10" s="28"/>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="29" t="s">
         <v>57</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1">
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>19</v>
       </c>
@@ -2538,20 +2554,18 @@
         <v>55</v>
       </c>
       <c r="C11" s="28"/>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="29" t="s">
+      <c r="E11" s="29" t="s">
         <v>51</v>
       </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
@@ -2567,12 +2581,12 @@
         <v>58</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>19</v>
       </c>
@@ -2588,12 +2602,12 @@
         <v>58</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>19</v>
       </c>
@@ -2609,12 +2623,12 @@
         <v>58</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>19</v>
       </c>
@@ -2630,12 +2644,12 @@
         <v>58</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>19</v>
       </c>
@@ -2651,12 +2665,12 @@
         <v>58</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
     </row>
-    <row r="17" spans="1:24" ht="15" customHeight="1">
+    <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>19</v>
       </c>
@@ -2672,12 +2686,12 @@
         <v>58</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" spans="1:24" ht="15" customHeight="1">
+    <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>19</v>
       </c>
@@ -2693,16 +2707,12 @@
         <v>58</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" ht="15" customHeight="1">
+        <v>60</v>
+      </c>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+    </row>
+    <row r="19" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>19</v>
       </c>
@@ -2718,16 +2728,16 @@
         <v>58</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I19" s="28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" ht="12.75" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>19</v>
       </c>
@@ -2739,16 +2749,20 @@
         <v>57</v>
       </c>
       <c r="E20" s="29"/>
-      <c r="F20" s="29" t="s">
-        <v>33</v>
+      <c r="F20" s="33" t="s">
+        <v>58</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-    </row>
-    <row r="21" spans="1:24" ht="18" customHeight="1">
+        <v>54</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>19</v>
       </c>
@@ -2756,7 +2770,7 @@
         <v>55</v>
       </c>
       <c r="C21" s="28"/>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="29" t="s">
         <v>57</v>
       </c>
       <c r="E21" s="29"/>
@@ -2764,12 +2778,12 @@
         <v>33</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
     </row>
-    <row r="22" spans="1:24" ht="18" customHeight="1">
+    <row r="22" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>19</v>
       </c>
@@ -2785,12 +2799,12 @@
         <v>33</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
     </row>
-    <row r="23" spans="1:24" ht="18" customHeight="1">
+    <row r="23" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>19</v>
       </c>
@@ -2806,12 +2820,12 @@
         <v>33</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
     </row>
-    <row r="24" spans="1:24" ht="18" customHeight="1">
+    <row r="24" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>19</v>
       </c>
@@ -2827,12 +2841,12 @@
         <v>33</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
     </row>
-    <row r="25" spans="1:24" ht="18" customHeight="1">
+    <row r="25" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>19</v>
       </c>
@@ -2848,12 +2862,12 @@
         <v>33</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
     </row>
-    <row r="26" spans="1:24" ht="18" customHeight="1">
+    <row r="26" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>19</v>
       </c>
@@ -2869,37 +2883,33 @@
         <v>33</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
     </row>
-    <row r="27" spans="1:24" ht="18" customHeight="1">
+    <row r="27" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="23"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="31"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" s="29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24">
+        <v>60</v>
+      </c>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+    </row>
+    <row r="28" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>19</v>
       </c>
@@ -2907,99 +2917,77 @@
         <v>55</v>
       </c>
       <c r="C28" s="23"/>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="31"/>
+      <c r="F28" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="39"/>
+      <c r="D29" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E29" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="19"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="29"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="23" t="s">
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="I28" s="29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24">
-      <c r="A29" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24"/>
-      <c r="U29" s="24"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="24"/>
-    </row>
-    <row r="30" spans="1:24">
-      <c r="A30" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-    </row>
-    <row r="31" spans="1:24">
+      <c r="I30" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" s="25" t="s">
+      <c r="C31" s="24" t="s">
         <v>51</v>
       </c>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
       <c r="F31" s="25"/>
       <c r="G31" s="25"/>
       <c r="H31" s="24"/>
@@ -3020,20 +3008,18 @@
       <c r="W31" s="24"/>
       <c r="X31" s="24"/>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>52</v>
-      </c>
+      <c r="C32" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
       <c r="F32" s="25"/>
       <c r="G32" s="25"/>
       <c r="H32" s="24"/>
@@ -3054,7 +3040,7 @@
       <c r="W32" s="24"/>
       <c r="X32" s="24"/>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
         <v>19</v>
       </c>
@@ -3088,7 +3074,7 @@
       <c r="W33" s="24"/>
       <c r="X33" s="24"/>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>19</v>
       </c>
@@ -3097,10 +3083,10 @@
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
@@ -3122,7 +3108,7 @@
       <c r="W34" s="24"/>
       <c r="X34" s="24"/>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>19</v>
       </c>
@@ -3131,10 +3117,10 @@
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F35" s="25"/>
       <c r="G35" s="25"/>
@@ -3156,7 +3142,7 @@
       <c r="W35" s="24"/>
       <c r="X35" s="24"/>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>19</v>
       </c>
@@ -3190,7 +3176,7 @@
       <c r="W36" s="24"/>
       <c r="X36" s="24"/>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>19</v>
       </c>
@@ -3202,7 +3188,7 @@
         <v>63</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
@@ -3224,7 +3210,7 @@
       <c r="W37" s="24"/>
       <c r="X37" s="24"/>
     </row>
-    <row r="38" spans="1:24">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>19</v>
       </c>
@@ -3258,7 +3244,7 @@
       <c r="W38" s="24"/>
       <c r="X38" s="24"/>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>19</v>
       </c>
@@ -3270,16 +3256,12 @@
         <v>63</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
-      <c r="H39" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="I39" s="27" t="s">
-        <v>29</v>
-      </c>
+      <c r="H39" s="24"/>
+      <c r="I39" s="26"/>
       <c r="J39" s="24"/>
       <c r="K39" s="24"/>
       <c r="L39" s="24"/>
@@ -3296,7 +3278,7 @@
       <c r="W39" s="24"/>
       <c r="X39" s="24"/>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>19</v>
       </c>
@@ -3305,7 +3287,7 @@
       </c>
       <c r="C40" s="24"/>
       <c r="D40" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E40" s="25" t="s">
         <v>51</v>
@@ -3330,7 +3312,7 @@
       <c r="W40" s="24"/>
       <c r="X40" s="24"/>
     </row>
-    <row r="41" spans="1:24">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>19</v>
       </c>
@@ -3339,17 +3321,17 @@
       </c>
       <c r="C41" s="24"/>
       <c r="D41" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F41" s="25"/>
       <c r="G41" s="25"/>
       <c r="H41" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="I41" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="I41" s="27" t="s">
         <v>29</v>
       </c>
       <c r="J41" s="24"/>
@@ -3368,7 +3350,7 @@
       <c r="W41" s="24"/>
       <c r="X41" s="24"/>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>19</v>
       </c>
@@ -3380,7 +3362,7 @@
         <v>65</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F42" s="25"/>
       <c r="G42" s="25"/>
@@ -3402,7 +3384,7 @@
       <c r="W42" s="24"/>
       <c r="X42" s="24"/>
     </row>
-    <row r="43" spans="1:24">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>19</v>
       </c>
@@ -3411,17 +3393,17 @@
       </c>
       <c r="C43" s="24"/>
       <c r="D43" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E43" s="32" t="s">
-        <v>54</v>
+        <v>65</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>56</v>
       </c>
       <c r="F43" s="25"/>
       <c r="G43" s="25"/>
       <c r="H43" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="I43" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" s="26" t="s">
         <v>29</v>
       </c>
       <c r="J43" s="24"/>
@@ -3440,84 +3422,124 @@
       <c r="W43" s="24"/>
       <c r="X43" s="24"/>
     </row>
-    <row r="44" spans="1:24">
-      <c r="A44" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="21" t="s">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="24"/>
+      <c r="D44" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
+      <c r="N44" s="24"/>
+      <c r="O44" s="24"/>
+      <c r="P44" s="24"/>
+      <c r="Q44" s="24"/>
+      <c r="R44" s="24"/>
+      <c r="S44" s="24"/>
+      <c r="T44" s="24"/>
+      <c r="U44" s="24"/>
+      <c r="V44" s="24"/>
+      <c r="W44" s="24"/>
+      <c r="X44" s="24"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A45" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="39"/>
+      <c r="D45" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-    </row>
-    <row r="45" spans="1:24">
-      <c r="A45" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45" s="21"/>
-      <c r="D45" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-    </row>
-    <row r="46" spans="1:24">
-      <c r="A46" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-    </row>
-    <row r="47" spans="1:24">
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="24"/>
+      <c r="N45" s="24"/>
+      <c r="O45" s="24"/>
+      <c r="P45" s="24"/>
+      <c r="Q45" s="24"/>
+      <c r="R45" s="24"/>
+      <c r="S45" s="24"/>
+      <c r="T45" s="24"/>
+      <c r="U45" s="24"/>
+      <c r="V45" s="24"/>
+      <c r="W45" s="24"/>
+      <c r="X45" s="24"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A46" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="24"/>
+      <c r="D46" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I46" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="24"/>
+      <c r="X46" s="24"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E47" s="20" t="s">
+      <c r="C47" s="21" t="s">
         <v>51</v>
       </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
       <c r="F47" s="20"/>
       <c r="G47" s="20"/>
       <c r="H47" s="21"/>
@@ -3526,7 +3548,7 @@
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>19</v>
       </c>
@@ -3538,7 +3560,7 @@
         <v>67</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="20"/>
@@ -3548,7 +3570,7 @@
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>19</v>
       </c>
@@ -3560,7 +3582,7 @@
         <v>67</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
@@ -3570,7 +3592,7 @@
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>19</v>
       </c>
@@ -3579,7 +3601,7 @@
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E50" s="20" t="s">
         <v>51</v>
@@ -3592,7 +3614,7 @@
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
@@ -3601,10 +3623,10 @@
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
@@ -3614,7 +3636,7 @@
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>19</v>
       </c>
@@ -3623,7 +3645,7 @@
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E52" s="20" t="s">
         <v>51</v>
@@ -3636,7 +3658,7 @@
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>19</v>
       </c>
@@ -3648,7 +3670,7 @@
         <v>68</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="20"/>
@@ -3658,7 +3680,7 @@
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>19</v>
       </c>
@@ -3670,7 +3692,7 @@
         <v>68</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F54" s="20"/>
       <c r="G54" s="20"/>
@@ -3680,7 +3702,7 @@
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
         <v>19</v>
       </c>
@@ -3692,7 +3714,7 @@
         <v>68</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="20"/>
@@ -3702,7 +3724,7 @@
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>19</v>
       </c>
@@ -3714,7 +3736,7 @@
         <v>68</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F56" s="20"/>
       <c r="G56" s="20"/>
@@ -3724,7 +3746,7 @@
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>19</v>
       </c>
@@ -3736,7 +3758,7 @@
         <v>68</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
@@ -3746,7 +3768,7 @@
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>19</v>
       </c>
@@ -3757,22 +3779,18 @@
       <c r="D58" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>56</v>
+      <c r="E58" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="F58" s="20"/>
       <c r="G58" s="20"/>
-      <c r="H58" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="I58" s="22" t="s">
-        <v>29</v>
-      </c>
+      <c r="H58" s="21"/>
+      <c r="I58" s="22"/>
       <c r="J58" s="21"/>
       <c r="K58" s="18"/>
       <c r="L58" s="18"/>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
         <v>19</v>
       </c>
@@ -3781,7 +3799,7 @@
       </c>
       <c r="C59" s="21"/>
       <c r="D59" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E59" s="20" t="s">
         <v>51</v>
@@ -3794,7 +3812,7 @@
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
         <v>19</v>
       </c>
@@ -3803,7 +3821,7 @@
       </c>
       <c r="C60" s="21"/>
       <c r="D60" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E60" s="20" t="s">
         <v>52</v>
@@ -3816,7 +3834,7 @@
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
         <v>19</v>
       </c>
@@ -3825,20 +3843,24 @@
       </c>
       <c r="C61" s="21"/>
       <c r="D61" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>51</v>
+        <v>68</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="F61" s="20"/>
       <c r="G61" s="20"/>
-      <c r="H61" s="21"/>
-      <c r="I61" s="22"/>
+      <c r="H61" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I61" s="22" t="s">
+        <v>29</v>
+      </c>
       <c r="J61" s="21"/>
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="21" t="s">
         <v>19</v>
       </c>
@@ -3850,7 +3872,7 @@
         <v>69</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F62" s="20"/>
       <c r="G62" s="20"/>
@@ -3860,7 +3882,7 @@
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
         <v>19</v>
       </c>
@@ -3872,21 +3894,17 @@
         <v>69</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="20"/>
-      <c r="H63" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="I63" s="22" t="s">
-        <v>29</v>
-      </c>
+      <c r="H63" s="21"/>
+      <c r="I63" s="22"/>
       <c r="J63" s="21"/>
       <c r="K63" s="18"/>
       <c r="L63" s="18"/>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
         <v>19</v>
       </c>
@@ -3895,147 +3913,129 @@
       </c>
       <c r="C64" s="21"/>
       <c r="D64" s="20" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F64" s="20"/>
       <c r="G64" s="20"/>
-      <c r="H64" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="I64" s="22" t="s">
-        <v>29</v>
-      </c>
+      <c r="H64" s="21"/>
+      <c r="I64" s="22"/>
       <c r="J64" s="21"/>
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
     </row>
-    <row r="65" spans="1:16">
-      <c r="A65" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="18"/>
-      <c r="I65" s="17"/>
-      <c r="J65" s="18"/>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65" s="21"/>
+      <c r="D65" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="22"/>
+      <c r="J65" s="21"/>
       <c r="K65" s="18"/>
       <c r="L65" s="18"/>
-      <c r="M65" s="18"/>
-      <c r="N65" s="18"/>
-      <c r="O65" s="18"/>
-      <c r="P65" s="18"/>
-    </row>
-    <row r="66" spans="1:16">
-      <c r="A66" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" s="18"/>
-      <c r="D66" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F66" s="35"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="18"/>
-      <c r="I66" s="17"/>
-      <c r="J66" s="18"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C66" s="21"/>
+      <c r="D66" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I66" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J66" s="21"/>
       <c r="K66" s="18"/>
       <c r="L66" s="18"/>
-      <c r="M66" s="18"/>
-      <c r="N66" s="18"/>
-      <c r="O66" s="18"/>
-      <c r="P66" s="18"/>
-    </row>
-    <row r="67" spans="1:16">
-      <c r="A67" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="18"/>
-      <c r="D67" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E67" s="19"/>
-      <c r="F67" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="G67" s="19" t="s">
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67" s="39"/>
+      <c r="D67" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E67" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="H67" s="18"/>
-      <c r="I67" s="17"/>
-      <c r="J67" s="18"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="21"/>
       <c r="K67" s="18"/>
       <c r="L67" s="18"/>
-      <c r="M67" s="18"/>
-      <c r="N67" s="18"/>
-      <c r="O67" s="18"/>
-      <c r="P67" s="18"/>
-    </row>
-    <row r="68" spans="1:16">
-      <c r="A68" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="18"/>
-      <c r="D68" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E68" s="19"/>
-      <c r="F68" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="G68" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="H68" s="18"/>
-      <c r="I68" s="17"/>
-      <c r="J68" s="18"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="21"/>
+      <c r="D68" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="I68" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J68" s="21"/>
       <c r="K68" s="18"/>
       <c r="L68" s="18"/>
-      <c r="M68" s="18"/>
-      <c r="N68" s="18"/>
-      <c r="O68" s="18"/>
-      <c r="P68" s="18"/>
-    </row>
-    <row r="69" spans="1:16">
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B69" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C69" s="18"/>
-      <c r="D69" s="19" t="s">
-        <v>41</v>
-      </c>
+      <c r="C69" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D69" s="19"/>
       <c r="E69" s="19"/>
-      <c r="F69" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G69" s="17" t="s">
-        <v>51</v>
-      </c>
+      <c r="F69" s="34"/>
+      <c r="G69" s="19"/>
       <c r="H69" s="18"/>
       <c r="I69" s="17"/>
       <c r="J69" s="18"/>
@@ -4046,7 +4046,7 @@
       <c r="O69" s="18"/>
       <c r="P69" s="18"/>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
         <v>19</v>
       </c>
@@ -4057,19 +4057,13 @@
       <c r="D70" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E70" s="19"/>
-      <c r="F70" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G70" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H70" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I70" s="17" t="s">
-        <v>29</v>
-      </c>
+      <c r="E70" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F70" s="35"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="17"/>
       <c r="J70" s="18"/>
       <c r="K70" s="18"/>
       <c r="L70" s="18"/>
@@ -4078,7 +4072,7 @@
       <c r="O70" s="18"/>
       <c r="P70" s="18"/>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
         <v>19</v>
       </c>
@@ -4087,13 +4081,15 @@
       </c>
       <c r="C71" s="18"/>
       <c r="D71" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E71" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E71" s="19"/>
+      <c r="F71" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="G71" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F71" s="34"/>
-      <c r="G71" s="19"/>
       <c r="H71" s="18"/>
       <c r="I71" s="17"/>
       <c r="J71" s="18"/>
@@ -4104,7 +4100,7 @@
       <c r="O71" s="18"/>
       <c r="P71" s="18"/>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
         <v>19</v>
       </c>
@@ -4113,13 +4109,15 @@
       </c>
       <c r="C72" s="18"/>
       <c r="D72" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E72" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F72" s="34"/>
-      <c r="G72" s="19"/>
+        <v>41</v>
+      </c>
+      <c r="E72" s="19"/>
+      <c r="F72" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="G72" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="H72" s="18"/>
       <c r="I72" s="17"/>
       <c r="J72" s="18"/>
@@ -4130,7 +4128,7 @@
       <c r="O72" s="18"/>
       <c r="P72" s="18"/>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
         <v>19</v>
       </c>
@@ -4139,13 +4137,15 @@
       </c>
       <c r="C73" s="18"/>
       <c r="D73" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E73" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E73" s="19"/>
+      <c r="F73" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="G73" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
       <c r="H73" s="18"/>
       <c r="I73" s="17"/>
       <c r="J73" s="18"/>
@@ -4156,7 +4156,7 @@
       <c r="O73" s="18"/>
       <c r="P73" s="18"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
         <v>19</v>
       </c>
@@ -4165,15 +4165,21 @@
       </c>
       <c r="C74" s="18"/>
       <c r="D74" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E74" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F74" s="19"/>
-      <c r="G74" s="19"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="17"/>
+        <v>41</v>
+      </c>
+      <c r="E74" s="19"/>
+      <c r="F74" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H74" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I74" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="J74" s="18"/>
       <c r="K74" s="18"/>
       <c r="L74" s="18"/>
@@ -4182,7 +4188,7 @@
       <c r="O74" s="18"/>
       <c r="P74" s="18"/>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
         <v>19</v>
       </c>
@@ -4196,7 +4202,7 @@
       <c r="E75" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F75" s="19"/>
+      <c r="F75" s="34"/>
       <c r="G75" s="19"/>
       <c r="H75" s="18"/>
       <c r="I75" s="17"/>
@@ -4208,7 +4214,7 @@
       <c r="O75" s="18"/>
       <c r="P75" s="18"/>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
         <v>19</v>
       </c>
@@ -4220,9 +4226,9 @@
         <v>73</v>
       </c>
       <c r="E76" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F76" s="19"/>
+        <v>59</v>
+      </c>
+      <c r="F76" s="34"/>
       <c r="G76" s="19"/>
       <c r="H76" s="18"/>
       <c r="I76" s="17"/>
@@ -4234,7 +4240,7 @@
       <c r="O76" s="18"/>
       <c r="P76" s="18"/>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>19</v>
       </c>
@@ -4260,7 +4266,7 @@
       <c r="O77" s="18"/>
       <c r="P77" s="18"/>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
         <v>19</v>
       </c>
@@ -4272,16 +4278,12 @@
         <v>73</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F78" s="19"/>
       <c r="G78" s="19"/>
-      <c r="H78" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I78" s="17" t="s">
-        <v>29</v>
-      </c>
+      <c r="H78" s="18"/>
+      <c r="I78" s="17"/>
       <c r="J78" s="18"/>
       <c r="K78" s="18"/>
       <c r="L78" s="18"/>
@@ -4290,7 +4292,7 @@
       <c r="O78" s="18"/>
       <c r="P78" s="18"/>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
         <v>19</v>
       </c>
@@ -4302,7 +4304,7 @@
         <v>73</v>
       </c>
       <c r="E79" s="19" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F79" s="19"/>
       <c r="G79" s="19"/>
@@ -4316,7 +4318,7 @@
       <c r="O79" s="18"/>
       <c r="P79" s="18"/>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
         <v>19</v>
       </c>
@@ -4325,19 +4327,15 @@
       </c>
       <c r="C80" s="18"/>
       <c r="D80" s="19" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="E80" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F80" s="19"/>
       <c r="G80" s="19"/>
-      <c r="H80" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="I80" s="17" t="s">
-        <v>29</v>
-      </c>
+      <c r="H80" s="18"/>
+      <c r="I80" s="17"/>
       <c r="J80" s="18"/>
       <c r="K80" s="18"/>
       <c r="L80" s="18"/>
@@ -4346,135 +4344,288 @@
       <c r="O80" s="18"/>
       <c r="P80" s="18"/>
     </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B81" s="2" t="s">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C81" s="18"/>
+      <c r="D81" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F81" s="19"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="17"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="18"/>
+      <c r="M81" s="18"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="18"/>
+      <c r="P81" s="18"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A82" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C82" s="18"/>
+      <c r="D82" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I82" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J82" s="18"/>
+      <c r="K82" s="18"/>
+      <c r="L82" s="18"/>
+      <c r="M82" s="18"/>
+      <c r="N82" s="18"/>
+      <c r="O82" s="18"/>
+      <c r="P82" s="18"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C83" s="18"/>
+      <c r="D83" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="17"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="18"/>
+      <c r="L83" s="18"/>
+      <c r="M83" s="18"/>
+      <c r="N83" s="18"/>
+      <c r="O83" s="18"/>
+      <c r="P83" s="18"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A84" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C84" s="39"/>
+      <c r="D84" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E84" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="F84" s="19"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="17"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="18"/>
+      <c r="M84" s="18"/>
+      <c r="N84" s="18"/>
+      <c r="O84" s="18"/>
+      <c r="P84" s="18"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C85" s="18"/>
+      <c r="D85" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I85" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J85" s="18"/>
+      <c r="K85" s="18"/>
+      <c r="L85" s="18"/>
+      <c r="M85" s="18"/>
+      <c r="N85" s="18"/>
+      <c r="O85" s="18"/>
+      <c r="P85" s="18"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B86" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C86" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D86" s="43"/>
+      <c r="E86" s="43"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="8"/>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="H87" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I81" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B82" s="2" t="s">
+      <c r="I87" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H88" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I82" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B83" s="2" t="s">
+      <c r="I88" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="H89" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I83" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B84" s="2" t="s">
+      <c r="I89" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="H90" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I84" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B85" s="2" t="s">
+      <c r="I90" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="H91" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I85" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B86" s="37" t="s">
+      <c r="I91" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A92" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B92" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="C86" s="37" t="s">
+      <c r="C92" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="D86" s="37"/>
-      <c r="E86" s="37"/>
-      <c r="F86" s="37"/>
-      <c r="G86" s="37"/>
-      <c r="H86" s="37"/>
-      <c r="I86" s="37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B87" s="37" t="s">
+      <c r="D92" s="37"/>
+      <c r="E92" s="37"/>
+      <c r="F92" s="37"/>
+      <c r="G92" s="37"/>
+      <c r="H92" s="37"/>
+      <c r="I92" s="37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A93" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B93" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="C87" s="37" t="s">
+      <c r="C93" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="D87" s="37"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="37"/>
-      <c r="G87" s="37"/>
-      <c r="H87" s="37" t="s">
+      <c r="D93" s="37"/>
+      <c r="E93" s="37"/>
+      <c r="F93" s="37"/>
+      <c r="G93" s="37"/>
+      <c r="H93" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="I87" s="37" t="s">
+      <c r="I93" s="37" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I87"/>
+  <autoFilter ref="A1:I93"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
CN0713: Ajuste de Esqueleto de guion para carga en GRECO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion13/EsqueletoGuion_CN_07_13_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion13/EsqueletoGuion_CN_07_13_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado07\guion13\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado07\guion13\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="3408" yWindow="1395" windowWidth="12244" windowHeight="9243" tabRatio="729" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CUADERNO DE ESTUDIO'!$A$1:$I$93</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'RECURSOS NUEVOS'!$A$1:$C$22</definedName>
   </definedNames>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="76">
   <si>
     <t>FICHA</t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>La relación entre la Biología y la Medicina</t>
-  </si>
-  <si>
-    <t>Cómo se hace un test químico</t>
   </si>
   <si>
     <t>Carencias y excesos de yodo y cloro</t>
@@ -1608,13 +1605,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
@@ -1622,7 +1619,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
@@ -1630,7 +1627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
@@ -1638,7 +1635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
@@ -1646,7 +1643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
@@ -1654,7 +1651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -1681,19 +1678,19 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
@@ -1713,7 +1710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>6</v>
       </c>
@@ -1739,16 +1736,16 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G12" s="10"/>
     </row>
   </sheetData>
@@ -1766,17 +1763,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1787,7 +1784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1798,7 +1795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1809,7 +1806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1820,7 +1817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1831,7 +1828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1842,9 +1839,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
@@ -1853,9 +1850,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1864,9 +1861,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -1875,9 +1872,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -1886,9 +1883,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
@@ -1897,9 +1894,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -1908,9 +1905,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
@@ -1919,9 +1916,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -1930,9 +1927,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
@@ -1941,9 +1938,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
@@ -1952,9 +1949,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -1963,9 +1960,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
@@ -1974,20 +1971,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>48</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -1996,9 +1993,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
@@ -2007,9 +2004,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -2041,17 +2038,17 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -2062,7 +2059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2073,7 +2070,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2084,7 +2081,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2095,7 +2092,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2106,7 +2103,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2117,7 +2114,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2128,183 +2125,183 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>46</v>
       </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
       <c r="C20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C28" s="6"/>
     </row>
   </sheetData>
@@ -2326,25 +2323,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D88" sqref="A87:D88"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="37.73046875" customWidth="1"/>
+    <col min="2" max="2" width="29.46484375" style="2" customWidth="1"/>
     <col min="3" max="3" width="21" style="2" customWidth="1"/>
-    <col min="4" max="4" width="59.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="52.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.1328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.1328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="52.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -2373,15 +2370,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -2389,15 +2386,15 @@
       <c r="G2" s="9"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2405,15 +2402,15 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2421,37 +2418,37 @@
       <c r="G4" s="9"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="39" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="41"/>
       <c r="D5" s="42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>53</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>54</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -2462,15 +2459,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
@@ -2481,15 +2478,15 @@
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>55</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>56</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -2504,19 +2501,19 @@
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
@@ -2525,19 +2522,19 @@
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
@@ -2546,189 +2543,189 @@
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="29" t="s">
         <v>58</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>59</v>
       </c>
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
     </row>
-    <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="28"/>
       <c r="D17" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
     </row>
-    <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="29"/>
       <c r="F18" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
     </row>
-    <row r="19" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H19" s="28" t="s">
         <v>26</v>
@@ -2737,23 +2734,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" s="29"/>
       <c r="F20" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H20" s="28" t="s">
         <v>32</v>
@@ -2762,170 +2759,170 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="29"/>
       <c r="F21" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
     </row>
-    <row r="22" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="29"/>
       <c r="F22" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
     </row>
-    <row r="23" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="29"/>
       <c r="F23" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
     </row>
-    <row r="24" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="28"/>
       <c r="D24" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="29"/>
       <c r="F24" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
     </row>
-    <row r="25" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="29"/>
       <c r="F25" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
     </row>
-    <row r="26" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="29"/>
       <c r="F26" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
     </row>
-    <row r="27" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="28"/>
       <c r="D27" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
     </row>
-    <row r="28" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E28" s="31"/>
       <c r="F28" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H28" s="23" t="s">
         <v>33</v>
@@ -2934,38 +2931,38 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="39" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="39"/>
       <c r="D29" s="38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="29"/>
       <c r="H29" s="23"/>
       <c r="I29" s="29"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A30" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="31" t="s">
         <v>53</v>
-      </c>
-      <c r="E30" s="31" t="s">
-        <v>54</v>
       </c>
       <c r="F30" s="31"/>
       <c r="G30" s="31"/>
@@ -2976,15 +2973,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
@@ -3008,15 +3005,15 @@
       <c r="W31" s="24"/>
       <c r="X31" s="24"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A32" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
@@ -3040,19 +3037,19 @@
       <c r="W32" s="24"/>
       <c r="X32" s="24"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A33" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" s="24"/>
       <c r="D33" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F33" s="25"/>
       <c r="G33" s="25"/>
@@ -3074,19 +3071,19 @@
       <c r="W33" s="24"/>
       <c r="X33" s="24"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A34" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
@@ -3108,19 +3105,19 @@
       <c r="W34" s="24"/>
       <c r="X34" s="24"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A35" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F35" s="25"/>
       <c r="G35" s="25"/>
@@ -3142,19 +3139,19 @@
       <c r="W35" s="24"/>
       <c r="X35" s="24"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A36" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="25"/>
@@ -3176,19 +3173,19 @@
       <c r="W36" s="24"/>
       <c r="X36" s="24"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A37" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="24"/>
       <c r="D37" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
@@ -3210,19 +3207,19 @@
       <c r="W37" s="24"/>
       <c r="X37" s="24"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A38" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" s="24"/>
       <c r="D38" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
@@ -3244,19 +3241,19 @@
       <c r="W38" s="24"/>
       <c r="X38" s="24"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A39" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="24"/>
       <c r="D39" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
@@ -3278,19 +3275,19 @@
       <c r="W39" s="24"/>
       <c r="X39" s="24"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A40" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" s="24"/>
       <c r="D40" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E40" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F40" s="25"/>
       <c r="G40" s="25"/>
@@ -3312,24 +3309,24 @@
       <c r="W40" s="24"/>
       <c r="X40" s="24"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A41" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="24"/>
       <c r="D41" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F41" s="25"/>
       <c r="G41" s="25"/>
       <c r="H41" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I41" s="27" t="s">
         <v>29</v>
@@ -3350,19 +3347,19 @@
       <c r="W41" s="24"/>
       <c r="X41" s="24"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A42" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F42" s="25"/>
       <c r="G42" s="25"/>
@@ -3384,24 +3381,24 @@
       <c r="W42" s="24"/>
       <c r="X42" s="24"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A43" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43" s="24"/>
       <c r="D43" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E43" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F43" s="25"/>
       <c r="G43" s="25"/>
       <c r="H43" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I43" s="26" t="s">
         <v>29</v>
@@ -3422,19 +3419,19 @@
       <c r="W43" s="24"/>
       <c r="X43" s="24"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A44" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E44" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
@@ -3456,19 +3453,19 @@
       <c r="W44" s="24"/>
       <c r="X44" s="24"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A45" s="39" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" s="39"/>
       <c r="D45" s="38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E45" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
@@ -3490,24 +3487,24 @@
       <c r="W45" s="24"/>
       <c r="X45" s="24"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A46" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="24"/>
       <c r="D46" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="32" t="s">
         <v>53</v>
-      </c>
-      <c r="E46" s="32" t="s">
-        <v>54</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25"/>
       <c r="H46" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I46" s="27" t="s">
         <v>29</v>
@@ -3528,15 +3525,15 @@
       <c r="W46" s="24"/>
       <c r="X46" s="24"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A47" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
@@ -3548,19 +3545,19 @@
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A48" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="20"/>
@@ -3570,19 +3567,19 @@
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
@@ -3592,19 +3589,19 @@
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F50" s="20"/>
       <c r="G50" s="20"/>
@@ -3614,19 +3611,19 @@
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
@@ -3636,19 +3633,19 @@
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F52" s="20"/>
       <c r="G52" s="20"/>
@@ -3658,19 +3655,19 @@
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="20"/>
@@ -3680,19 +3677,19 @@
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F54" s="20"/>
       <c r="G54" s="20"/>
@@ -3702,19 +3699,19 @@
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F55" s="20"/>
       <c r="G55" s="20"/>
@@ -3724,19 +3721,19 @@
       <c r="K55" s="18"/>
       <c r="L55" s="18"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F56" s="20"/>
       <c r="G56" s="20"/>
@@ -3746,19 +3743,19 @@
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
@@ -3768,19 +3765,19 @@
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="21"/>
       <c r="D58" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F58" s="20"/>
       <c r="G58" s="20"/>
@@ -3790,19 +3787,19 @@
       <c r="K58" s="18"/>
       <c r="L58" s="18"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A59" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" s="21"/>
       <c r="D59" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E59" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F59" s="20"/>
       <c r="G59" s="20"/>
@@ -3812,19 +3809,19 @@
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" s="21"/>
       <c r="D60" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E60" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F60" s="20"/>
       <c r="G60" s="20"/>
@@ -3834,24 +3831,24 @@
       <c r="K60" s="18"/>
       <c r="L60" s="18"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A61" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C61" s="21"/>
       <c r="D61" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F61" s="20"/>
       <c r="G61" s="20"/>
       <c r="H61" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I61" s="22" t="s">
         <v>29</v>
@@ -3860,19 +3857,19 @@
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" s="21"/>
       <c r="D62" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F62" s="20"/>
       <c r="G62" s="20"/>
@@ -3882,19 +3879,19 @@
       <c r="K62" s="18"/>
       <c r="L62" s="18"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63" s="21"/>
       <c r="D63" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="20"/>
@@ -3904,19 +3901,19 @@
       <c r="K63" s="18"/>
       <c r="L63" s="18"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C64" s="21"/>
       <c r="D64" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F64" s="20"/>
       <c r="G64" s="20"/>
@@ -3926,19 +3923,19 @@
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A65" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C65" s="21"/>
       <c r="D65" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E65" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F65" s="20"/>
       <c r="G65" s="20"/>
@@ -3948,24 +3945,24 @@
       <c r="K65" s="18"/>
       <c r="L65" s="18"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A66" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66" s="21"/>
       <c r="D66" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E66" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F66" s="20"/>
       <c r="G66" s="20"/>
       <c r="H66" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I66" s="22" t="s">
         <v>29</v>
@@ -3974,19 +3971,19 @@
       <c r="K66" s="18"/>
       <c r="L66" s="18"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A67" s="39" t="s">
         <v>19</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C67" s="39"/>
       <c r="D67" s="38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E67" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F67" s="20"/>
       <c r="G67" s="20"/>
@@ -3996,24 +3993,24 @@
       <c r="K67" s="18"/>
       <c r="L67" s="18"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A68" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C68" s="21"/>
       <c r="D68" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E68" s="20" t="s">
         <v>53</v>
-      </c>
-      <c r="E68" s="20" t="s">
-        <v>54</v>
       </c>
       <c r="F68" s="20"/>
       <c r="G68" s="20"/>
       <c r="H68" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I68" s="22" t="s">
         <v>29</v>
@@ -4022,15 +4019,15 @@
       <c r="K68" s="18"/>
       <c r="L68" s="18"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A69" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D69" s="19"/>
       <c r="E69" s="19"/>
@@ -4046,19 +4043,19 @@
       <c r="O69" s="18"/>
       <c r="P69" s="18"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A70" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F70" s="35"/>
       <c r="G70" s="19"/>
@@ -4072,23 +4069,23 @@
       <c r="O70" s="18"/>
       <c r="P70" s="18"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A71" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C71" s="18"/>
       <c r="D71" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E71" s="19"/>
       <c r="F71" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G71" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H71" s="18"/>
       <c r="I71" s="17"/>
@@ -4100,23 +4097,23 @@
       <c r="O71" s="18"/>
       <c r="P71" s="18"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A72" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C72" s="18"/>
       <c r="D72" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E72" s="19"/>
       <c r="F72" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G72" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H72" s="18"/>
       <c r="I72" s="17"/>
@@ -4128,23 +4125,23 @@
       <c r="O72" s="18"/>
       <c r="P72" s="18"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A73" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C73" s="18"/>
       <c r="D73" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E73" s="19"/>
       <c r="F73" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G73" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H73" s="18"/>
       <c r="I73" s="17"/>
@@ -4156,26 +4153,26 @@
       <c r="O73" s="18"/>
       <c r="P73" s="18"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A74" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C74" s="18"/>
       <c r="D74" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E74" s="19"/>
       <c r="F74" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G74" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H74" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I74" s="17" t="s">
         <v>29</v>
@@ -4188,19 +4185,19 @@
       <c r="O74" s="18"/>
       <c r="P74" s="18"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A75" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C75" s="18"/>
       <c r="D75" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E75" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F75" s="34"/>
       <c r="G75" s="19"/>
@@ -4214,19 +4211,19 @@
       <c r="O75" s="18"/>
       <c r="P75" s="18"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A76" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C76" s="18"/>
       <c r="D76" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E76" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F76" s="34"/>
       <c r="G76" s="19"/>
@@ -4240,19 +4237,19 @@
       <c r="O76" s="18"/>
       <c r="P76" s="18"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A77" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C77" s="18"/>
       <c r="D77" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F77" s="19"/>
       <c r="G77" s="19"/>
@@ -4266,19 +4263,19 @@
       <c r="O77" s="18"/>
       <c r="P77" s="18"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A78" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F78" s="19"/>
       <c r="G78" s="19"/>
@@ -4292,19 +4289,19 @@
       <c r="O78" s="18"/>
       <c r="P78" s="18"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A79" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C79" s="18"/>
       <c r="D79" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E79" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F79" s="19"/>
       <c r="G79" s="19"/>
@@ -4318,19 +4315,19 @@
       <c r="O79" s="18"/>
       <c r="P79" s="18"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A80" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C80" s="18"/>
       <c r="D80" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E80" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F80" s="19"/>
       <c r="G80" s="19"/>
@@ -4344,19 +4341,19 @@
       <c r="O80" s="18"/>
       <c r="P80" s="18"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A81" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C81" s="18"/>
       <c r="D81" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E81" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F81" s="19"/>
       <c r="G81" s="19"/>
@@ -4370,24 +4367,24 @@
       <c r="O81" s="18"/>
       <c r="P81" s="18"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A82" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C82" s="18"/>
       <c r="D82" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E82" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F82" s="19"/>
       <c r="G82" s="19"/>
       <c r="H82" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I82" s="17" t="s">
         <v>29</v>
@@ -4400,19 +4397,19 @@
       <c r="O82" s="18"/>
       <c r="P82" s="18"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A83" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C83" s="18"/>
       <c r="D83" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F83" s="19"/>
       <c r="G83" s="19"/>
@@ -4426,19 +4423,19 @@
       <c r="O83" s="18"/>
       <c r="P83" s="18"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A84" s="39" t="s">
         <v>19</v>
       </c>
       <c r="B84" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C84" s="39"/>
       <c r="D84" s="38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E84" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F84" s="19"/>
       <c r="G84" s="19"/>
@@ -4452,24 +4449,24 @@
       <c r="O84" s="18"/>
       <c r="P84" s="18"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A85" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C85" s="18"/>
       <c r="D85" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E85" s="19" t="s">
         <v>53</v>
-      </c>
-      <c r="E85" s="19" t="s">
-        <v>54</v>
       </c>
       <c r="F85" s="19"/>
       <c r="G85" s="19"/>
       <c r="H85" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I85" s="17" t="s">
         <v>29</v>
@@ -4482,115 +4479,115 @@
       <c r="O85" s="18"/>
       <c r="P85" s="18"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A86" s="39" t="s">
         <v>19</v>
       </c>
       <c r="B86" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C86" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D86" s="43"/>
       <c r="E86" s="43"/>
       <c r="H86" s="2"/>
       <c r="I86" s="8"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H87" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I87" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A88" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H88" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I87" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H88" s="2" t="s">
+      <c r="I88" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A89" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H89" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I88" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H89" s="2" t="s">
+      <c r="I89" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A90" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H90" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I89" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H90" s="2" t="s">
+      <c r="I90" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A91" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H91" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I90" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H91" s="2" t="s">
+      <c r="I91" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A92" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B92" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C92" s="37" t="s">
         <v>48</v>
-      </c>
-      <c r="I91" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A92" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B92" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C92" s="37" t="s">
-        <v>49</v>
       </c>
       <c r="D92" s="37"/>
       <c r="E92" s="37"/>
@@ -4601,22 +4598,22 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A93" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B93" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C93" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D93" s="37"/>
       <c r="E93" s="37"/>
       <c r="F93" s="37"/>
       <c r="G93" s="37"/>
       <c r="H93" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I93" s="37" t="s">
         <v>29</v>

</xml_diff>